<commit_message>
update list of variable names
</commit_message>
<xml_diff>
--- a/CrossScale Emergence/Variable_Name_Metadata.xlsx
+++ b/CrossScale Emergence/Variable_Name_Metadata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farrellk\Desktop\R\ProjectEDDIE\Lake Modeling Module_2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KFarrell\Desktop\R\ProjectEDDIE\CrossScale Emergence\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>File name</t>
   </si>
@@ -35,27 +35,9 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>field_data.csv</t>
-  </si>
-  <si>
-    <t>DateTime</t>
-  </si>
-  <si>
-    <t>Depth</t>
-  </si>
-  <si>
-    <t>temp</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
-    <t>yyyy-mm-dd</t>
-  </si>
-  <si>
-    <t>daily</t>
-  </si>
-  <si>
     <t>°C</t>
   </si>
   <si>
@@ -89,24 +71,12 @@
     <t>Snow</t>
   </si>
   <si>
-    <t>yyyy-mm-dd hh:mm</t>
-  </si>
-  <si>
     <t>hourly</t>
   </si>
   <si>
     <t>meters/day</t>
   </si>
   <si>
-    <t>Convert from mm/d by multiplying by 0.001</t>
-  </si>
-  <si>
-    <t>meters</t>
-  </si>
-  <si>
-    <t>Lake depth</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -119,23 +89,204 @@
     <t>Description</t>
   </si>
   <si>
-    <t>W/m2</t>
-  </si>
-  <si>
     <t>WindSpeed</t>
   </si>
   <si>
     <t>decimal ≥ 0</t>
+  </si>
+  <si>
+    <t>inflow.csv</t>
+  </si>
+  <si>
+    <t>FLOW</t>
+  </si>
+  <si>
+    <t>SALT</t>
+  </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>OGM_don</t>
+  </si>
+  <si>
+    <t>NIT_nit</t>
+  </si>
+  <si>
+    <t>NIT_amm</t>
+  </si>
+  <si>
+    <t>PHS_frp</t>
+  </si>
+  <si>
+    <t>outflow.csv</t>
+  </si>
+  <si>
+    <t>water flow into lake</t>
+  </si>
+  <si>
+    <t>water flow out of lake</t>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/s</t>
+    </r>
+  </si>
+  <si>
+    <t>salt concentration in inflow water</t>
+  </si>
+  <si>
+    <t>water temperature</t>
+  </si>
+  <si>
+    <t>dissolved organic nitrogen concentration in inflow water</t>
+  </si>
+  <si>
+    <t>nitrate concentration in inflow water</t>
+  </si>
+  <si>
+    <t>ammonium concentration in inflow water</t>
+  </si>
+  <si>
+    <t>filterable reactive phosphorus concentration in inflow water</t>
+  </si>
+  <si>
+    <t>shortwave radiation</t>
+  </si>
+  <si>
+    <t>longwave radiation</t>
+  </si>
+  <si>
+    <t>Air temperature</t>
+  </si>
+  <si>
+    <t>relative humidity</t>
+  </si>
+  <si>
+    <t>daily snow</t>
+  </si>
+  <si>
+    <r>
+      <t>W/m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>yyyy-mm-dd hh:mm:ss</t>
+  </si>
+  <si>
+    <t>parts per thousand</t>
+  </si>
+  <si>
+    <r>
+      <t>mmol N/m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>mmol P/m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <t>Unit Conversion Notes</t>
+  </si>
+  <si>
+    <t>daily rain</t>
+  </si>
+  <si>
+    <t>convert from mm/day by multiplying by 0.001</t>
+  </si>
+  <si>
+    <t>convert from cubic feet per second by multiplying by 0.0283</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">convert </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mg/L by multiplying by 32.29</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +308,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -166,7 +332,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -174,16 +340,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -193,9 +365,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,236 +690,407 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="10">
+        <v>36587</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>-2.5139999999999998</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>308.887</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>20.05</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>38.619999999999997</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>1.87</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>5.9199999999999997E-4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5">
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="10">
         <v>36587</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="11" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E11">
+        <v>2.38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="6">
-        <v>17.64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="5">
-        <v>36587</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>-2.5139999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>308.887</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8">
-        <v>20.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>38.619999999999997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10">
-        <v>1.87</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11">
-        <v>5.9199999999999997E-4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
       <c r="C12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
+        <v>48</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="E12">
         <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>17.2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>92.601500000000001</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>926.01530000000002</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>14.084899999999999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.79179641999999995</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="10">
+        <v>36587</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19">
+        <v>1.41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>